<commit_message>
chore: add #active to test setting table
To reproduce the bug
</commit_message>
<xml_diff>
--- a/GameData/ValidExamples.xlsx
+++ b/GameData/ValidExamples.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ValidExampleData" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="65">
   <si>
     <t xml:space="preserve">namespace=TestGame</t>
   </si>
@@ -493,8 +493,8 @@
   </sheetPr>
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.03515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -643,10 +643,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G19" activeCellId="0" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.03515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -663,297 +663,375 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="3" t="n">
-        <v>200</v>
+    <row r="2" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4"/>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="3" t="n">
-        <v>10005</v>
+      <c r="D3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="3" t="n">
+        <v>200</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="3" t="n">
-        <v>0</v>
+      <c r="D4" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="3" t="n">
+        <v>10005</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="3" t="n">
-        <v>5000</v>
+      <c r="D5" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="3" t="n">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B7" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="3" t="n">
+      <c r="C7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="3" t="n">
         <v>10000</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="3" t="n">
-        <v>8000</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="3" t="n">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B9" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="3" t="n">
+      <c r="C9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="3" t="n">
         <v>2000</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="6" t="s">
+    <row r="10" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B10" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="3" t="n">
+      <c r="C10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="3" t="n">
         <v>80</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="6" t="s">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B11" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="3" t="n">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>42</v>
-      </c>
       <c r="C11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="3" t="n">
+      <c r="D11" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="3" t="n">
         <v>5000</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="3" t="n">
-        <v>1000</v>
+      <c r="D12" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="3" t="n">
+        <v>5000</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="3" t="n">
-        <v>30000</v>
+      <c r="D13" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="3" t="n">
+        <v>1000</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="3" t="n">
-        <v>10000</v>
+      <c r="D14" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="3" t="n">
+        <v>30000</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="3" t="n">
-        <v>1000</v>
+      <c r="D15" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="3" t="n">
+        <v>10000</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="3" t="n">
-        <v>2000</v>
+      <c r="D16" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="3" t="n">
+        <v>1000</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="3" t="n">
-        <v>3000</v>
+      <c r="D17" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="3" t="n">
+        <v>2000</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="3" t="n">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B19" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" s="3" t="n">
+      <c r="C19" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="3" t="n">
         <v>1000</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="6" t="s">
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B20" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" s="3" t="n">
+      <c r="C20" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" s="3" t="n">
         <v>20</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="6" t="s">
+    <row r="21" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B21" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D20" s="3" t="n">
+      <c r="C21" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" s="3" t="n">
         <v>2000</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D21" s="3" t="n">
-        <v>165</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" s="3" t="n">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B23" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D22" s="3" t="n">
+      <c r="C23" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23" s="3" t="n">
         <v>200</v>
       </c>
     </row>

</xml_diff>